<commit_message>
Fixed the template and added code to write bit fields to doc
</commit_message>
<xml_diff>
--- a/DMS/Data/Loose fill form .xlsx
+++ b/DMS/Data/Loose fill form .xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejaz.s\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -732,9 +727,6 @@
     <t>Label:Location|Row:6|Column:0|ColumnSpan:2|Values:On the top of ceiling lining~On the top of ceiling lining,On the top of framework~On the top of framework|WindowOnly:True</t>
   </si>
   <si>
-    <t>Label:Result|Row:8|Column:0|ColumnSpan:2|Attributes:Distance,Direction,Above,Location|GridOnly:True</t>
-  </si>
-  <si>
     <t>{{ConsultantName}}</t>
   </si>
   <si>
@@ -1024,15 +1016,25 @@
   </si>
   <si>
     <t>[[Hotwaterunit]]</t>
+  </si>
+  <si>
+    <t>Label:Sample Location|Row:8|Column:0|ColumnSpan:2|Attributes:Distance,Direction,Above,Location|GridOnly:True</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="15">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1322,130 +1324,130 @@
   </borders>
   <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1460,21 +1462,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1482,25 +1484,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1515,27 +1517,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2069,7 +2074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:R92"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
@@ -2284,7 +2289,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="17.25">
+    <row r="18" spans="2:11">
       <c r="B18" s="10"/>
       <c r="C18" s="27" t="s">
         <v>31</v>
@@ -2312,7 +2317,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="2:11" ht="17.25">
+    <row r="20" spans="2:11">
       <c r="B20" s="10"/>
       <c r="C20" s="27" t="s">
         <v>32</v>
@@ -2340,7 +2345,7 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="2:11" ht="17.25">
+    <row r="22" spans="2:11">
       <c r="B22" s="10"/>
       <c r="C22" s="27" t="s">
         <v>33</v>
@@ -2368,7 +2373,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="2:11" ht="17.25">
+    <row r="24" spans="2:11">
       <c r="B24" s="10"/>
       <c r="C24" s="27" t="s">
         <v>34</v>
@@ -2396,7 +2401,7 @@
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="2:11" ht="17.25">
+    <row r="26" spans="2:11">
       <c r="B26" s="10"/>
       <c r="C26" s="27" t="s">
         <v>18</v>
@@ -2424,7 +2429,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="2:11" ht="17.25">
+    <row r="28" spans="2:11">
       <c r="B28" s="10"/>
       <c r="C28" s="29" t="s">
         <v>17</v>
@@ -2440,7 +2445,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="2:11" ht="17.25">
+    <row r="29" spans="2:11">
       <c r="B29" s="10"/>
       <c r="C29" s="26" t="s">
         <v>35</v>
@@ -2466,7 +2471,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="2:11" ht="17.25">
+    <row r="31" spans="2:11">
       <c r="B31" s="10"/>
       <c r="C31" s="26" t="s">
         <v>36</v>
@@ -2494,7 +2499,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="2:9" ht="17.25">
+    <row r="33" spans="2:9">
       <c r="B33" s="10"/>
       <c r="C33" s="26" t="s">
         <v>18</v>
@@ -2522,7 +2527,7 @@
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="2:9" ht="17.25">
+    <row r="35" spans="2:9">
       <c r="B35" s="10"/>
       <c r="C35" s="29" t="s">
         <v>18</v>
@@ -2538,7 +2543,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="2:9" ht="17.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="10"/>
       <c r="C36" s="27" t="s">
         <v>37</v>
@@ -2570,7 +2575,7 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="2:9" ht="17.25">
+    <row r="38" spans="2:9">
       <c r="B38" s="10"/>
       <c r="C38" s="27" t="s">
         <v>38</v>
@@ -2596,7 +2601,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
     </row>
-    <row r="40" spans="2:9" ht="17.25">
+    <row r="40" spans="2:9">
       <c r="B40" s="10"/>
       <c r="C40" s="27" t="s">
         <v>39</v>
@@ -2624,7 +2629,7 @@
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
     </row>
-    <row r="42" spans="2:9" ht="17.25">
+    <row r="42" spans="2:9">
       <c r="B42" s="10"/>
       <c r="C42" s="27" t="s">
         <v>18</v>
@@ -2652,7 +2657,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" spans="2:9" ht="17.25">
+    <row r="44" spans="2:9">
       <c r="B44" s="10"/>
       <c r="C44" s="27"/>
       <c r="D44" s="6"/>
@@ -2708,7 +2713,7 @@
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
     </row>
-    <row r="49" spans="2:18" ht="17.25">
+    <row r="49" spans="2:18">
       <c r="B49" s="10"/>
       <c r="C49" s="27"/>
       <c r="D49" s="6"/>
@@ -2732,7 +2737,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
     </row>
-    <row r="51" spans="2:18" ht="17.25">
+    <row r="51" spans="2:18">
       <c r="B51" s="10"/>
       <c r="C51" s="27"/>
       <c r="D51" s="6"/>
@@ -2756,7 +2761,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
     </row>
-    <row r="53" spans="2:18" ht="17.25">
+    <row r="53" spans="2:18">
       <c r="B53" s="10"/>
       <c r="C53" s="27"/>
       <c r="D53" s="6"/>
@@ -2780,7 +2785,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
     </row>
-    <row r="55" spans="2:18" ht="17.25">
+    <row r="55" spans="2:18">
       <c r="B55" s="10"/>
       <c r="C55" s="27"/>
       <c r="D55" s="6"/>
@@ -2804,7 +2809,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
     </row>
-    <row r="57" spans="2:18" ht="17.25">
+    <row r="57" spans="2:18">
       <c r="B57" s="10"/>
       <c r="C57" s="27"/>
       <c r="D57" s="6"/>
@@ -2828,7 +2833,7 @@
       <c r="H58" s="11"/>
       <c r="I58" s="11"/>
     </row>
-    <row r="59" spans="2:18" ht="17.25">
+    <row r="59" spans="2:18">
       <c r="B59" s="10"/>
       <c r="C59" s="30"/>
       <c r="D59" s="14"/>
@@ -3411,11 +3416,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:D61"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection sqref="A1:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -3437,7 +3442,7 @@
         <v>93</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
@@ -3451,7 +3456,7 @@
         <v>95</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
@@ -3465,7 +3470,7 @@
         <v>97</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
@@ -3479,7 +3484,7 @@
         <v>99</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
@@ -3493,7 +3498,7 @@
         <v>101</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
@@ -3507,11 +3512,11 @@
         <v>103</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="54" t="s">
         <v>104</v>
       </c>
       <c r="B7" s="50" t="s">
@@ -3521,7 +3526,7 @@
         <v>105</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
@@ -3535,7 +3540,7 @@
         <v>170</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
@@ -3549,7 +3554,7 @@
         <v>173</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
@@ -3563,7 +3568,7 @@
         <v>109</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
@@ -3577,7 +3582,7 @@
         <v>120</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
@@ -3588,10 +3593,10 @@
         <v>112</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
@@ -3602,10 +3607,10 @@
         <v>112</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
@@ -3616,10 +3621,10 @@
         <v>112</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
@@ -3630,10 +3635,10 @@
         <v>112</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
@@ -3644,10 +3649,10 @@
         <v>112</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
@@ -3661,7 +3666,7 @@
         <v>121</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
@@ -3672,10 +3677,10 @@
         <v>112</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
@@ -3686,10 +3691,10 @@
         <v>112</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
@@ -3700,10 +3705,10 @@
         <v>112</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
@@ -3717,7 +3722,7 @@
         <v>172</v>
       </c>
       <c r="D21" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
@@ -3728,10 +3733,10 @@
         <v>112</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
@@ -3742,10 +3747,10 @@
         <v>112</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
@@ -3756,10 +3761,10 @@
         <v>112</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
@@ -3770,10 +3775,10 @@
         <v>112</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
@@ -3787,7 +3792,7 @@
         <v>110</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
@@ -3798,10 +3803,10 @@
         <v>108</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
@@ -3812,10 +3817,10 @@
         <v>112</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
@@ -3826,10 +3831,10 @@
         <v>112</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D29" s="53" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
@@ -3840,10 +3845,10 @@
         <v>112</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D30" s="53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
@@ -3854,24 +3859,24 @@
         <v>112</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D31" s="53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B32" s="51" t="s">
         <v>112</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D32" s="53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1">
@@ -3882,10 +3887,10 @@
         <v>112</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D33" s="53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
@@ -3899,7 +3904,7 @@
         <v>142</v>
       </c>
       <c r="D34" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1">
@@ -3910,10 +3915,10 @@
         <v>112</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D35" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
@@ -3924,10 +3929,10 @@
         <v>112</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D36" s="53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1">
@@ -3938,10 +3943,10 @@
         <v>112</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D37" s="53" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1">
@@ -3952,10 +3957,10 @@
         <v>112</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D38" s="53" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1">
@@ -3966,10 +3971,10 @@
         <v>112</v>
       </c>
       <c r="C39" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D39" s="53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1">
@@ -3983,7 +3988,7 @@
         <v>143</v>
       </c>
       <c r="D40" s="50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1">
@@ -3994,10 +3999,10 @@
         <v>112</v>
       </c>
       <c r="C41" s="50" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D41" s="53" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
@@ -4008,10 +4013,10 @@
         <v>112</v>
       </c>
       <c r="C42" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D42" s="53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1">
@@ -4022,10 +4027,10 @@
         <v>112</v>
       </c>
       <c r="C43" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D43" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1">
@@ -4039,7 +4044,7 @@
         <v>144</v>
       </c>
       <c r="D44" s="50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1">
@@ -4050,24 +4055,24 @@
         <v>112</v>
       </c>
       <c r="C45" s="50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D45" s="53" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B46" s="51" t="s">
         <v>112</v>
       </c>
       <c r="C46" s="50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D46" s="53" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
@@ -4078,10 +4083,10 @@
         <v>112</v>
       </c>
       <c r="C47" s="50" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D47" s="53" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1">
@@ -4092,10 +4097,10 @@
         <v>112</v>
       </c>
       <c r="C48" s="50" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D48" s="53" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1">
@@ -4106,10 +4111,10 @@
         <v>112</v>
       </c>
       <c r="C49" s="50" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D49" s="53" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
@@ -4120,10 +4125,10 @@
         <v>112</v>
       </c>
       <c r="C50" s="50" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D50" s="53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1">
@@ -4134,10 +4139,10 @@
         <v>146</v>
       </c>
       <c r="C51" s="53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D51" s="53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1">
@@ -4151,7 +4156,7 @@
         <v>160</v>
       </c>
       <c r="D52" s="50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1">
@@ -4165,7 +4170,7 @@
         <v>147</v>
       </c>
       <c r="D53" s="53" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1">
@@ -4179,7 +4184,7 @@
         <v>156</v>
       </c>
       <c r="D54" s="53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1">
@@ -4193,7 +4198,7 @@
         <v>174</v>
       </c>
       <c r="D55" s="53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
@@ -4207,7 +4212,7 @@
         <v>175</v>
       </c>
       <c r="D56" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
@@ -4221,7 +4226,7 @@
         <v>176</v>
       </c>
       <c r="D57" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
@@ -4235,7 +4240,7 @@
         <v>177</v>
       </c>
       <c r="D58" s="50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1">
@@ -4249,39 +4254,39 @@
         <v>178</v>
       </c>
       <c r="D59" s="50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B60" s="51" t="s">
-        <v>146</v>
-      </c>
-      <c r="C60" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="D60" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="D60" s="53" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B61" s="51" t="s">
-        <v>148</v>
-      </c>
-      <c r="C61" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="D61" s="53" t="s">
-        <v>198</v>
+        <v>146</v>
+      </c>
+      <c r="C61" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="D61" s="50" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576 A1:A1048576">
+  <conditionalFormatting sqref="A1:A1048576 D1:D1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed issues in repeater doc replacement. Fixed some issues in the template. Modified repeater attribute from to {{RepeaterName.AttributeName}}
</commit_message>
<xml_diff>
--- a/DMS/Data/Loose fill form .xlsx
+++ b/DMS/Data/Loose fill form .xlsx
@@ -670,9 +670,6 @@
     <t>Repeater</t>
   </si>
   <si>
-    <t>Label:Sample Details|Row:31|Column:0|ColumnSpan:2</t>
-  </si>
-  <si>
     <t>Sample.SampleId</t>
   </si>
   <si>
@@ -715,12 +712,6 @@
     <t>Label:Sample location|Row:2|Column:0|ColumnSpan:1|Value:Sample location|WindowOnly:True</t>
   </si>
   <si>
-    <t>Label:Distance|Row:3|Column:0|ColumnSpan:2|Placeholder:|Prefix:|Suffix:meters|WindowOnly:True</t>
-  </si>
-  <si>
-    <t>Label:Direction|Row:4|Column:0|ColumnSpan:2|Placeholder:|Prefix:|Suffix:of manhole|WindowOnly:True</t>
-  </si>
-  <si>
     <t>Label:Above|Row:5|Column:0|ColumnSpan:2|Placeholder:|Prefix:|Suffix:|WindowOnly:True</t>
   </si>
   <si>
@@ -1019,15 +1010,31 @@
   </si>
   <si>
     <t>Label:Sample Location|Row:8|Column:0|ColumnSpan:2|Attributes:Distance,Direction,Above,Location|GridOnly:True</t>
+  </si>
+  <si>
+    <t>Label:Sample Details|Row:31|Column:0|ColumnSpan:2|CountLabel:No. Of Samples collected</t>
+  </si>
+  <si>
+    <t>Label:Distance|Row:3|Column:0|ColumnSpan:2|Placeholder:|Prefix:|Suffix: meters|WindowOnly:True</t>
+  </si>
+  <si>
+    <t>Label:Direction|Row:4|Column:0|ColumnSpan:2|Placeholder:|Prefix:|Suffix: of manhole|WindowOnly:True</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1324,130 +1331,130 @@
   </borders>
   <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1462,21 +1469,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1484,25 +1491,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1517,27 +1524,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2077,8 +2087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:R92"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView showGridLines="0" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3419,8 +3429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection sqref="A1:C61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -3442,7 +3452,7 @@
         <v>93</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
@@ -3456,7 +3466,7 @@
         <v>95</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
@@ -3464,13 +3474,13 @@
         <v>96</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>97</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
@@ -3478,13 +3488,13 @@
         <v>98</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>99</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
@@ -3498,7 +3508,7 @@
         <v>101</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
@@ -3512,7 +3522,7 @@
         <v>103</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
@@ -3525,8 +3535,8 @@
       <c r="C7" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="53" t="s">
-        <v>185</v>
+      <c r="D7" s="55" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
@@ -3534,13 +3544,13 @@
         <v>106</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
@@ -3551,10 +3561,10 @@
         <v>108</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
@@ -3568,7 +3578,7 @@
         <v>109</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
@@ -3582,7 +3592,7 @@
         <v>120</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
@@ -3593,10 +3603,10 @@
         <v>112</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
@@ -3607,10 +3617,10 @@
         <v>112</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
@@ -3621,10 +3631,10 @@
         <v>112</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
@@ -3635,10 +3645,10 @@
         <v>112</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
@@ -3649,10 +3659,10 @@
         <v>112</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
@@ -3666,7 +3676,7 @@
         <v>121</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
@@ -3677,10 +3687,10 @@
         <v>112</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
@@ -3691,10 +3701,10 @@
         <v>112</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
@@ -3705,10 +3715,10 @@
         <v>112</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
@@ -3719,10 +3729,10 @@
         <v>108</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" s="50" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
@@ -3733,10 +3743,10 @@
         <v>112</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
@@ -3747,10 +3757,10 @@
         <v>112</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
@@ -3761,10 +3771,10 @@
         <v>112</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
@@ -3775,10 +3785,10 @@
         <v>112</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
@@ -3792,7 +3802,7 @@
         <v>110</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
@@ -3803,10 +3813,10 @@
         <v>108</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
@@ -3817,10 +3827,10 @@
         <v>112</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
@@ -3831,10 +3841,10 @@
         <v>112</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D29" s="53" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
@@ -3845,10 +3855,10 @@
         <v>112</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D30" s="53" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
@@ -3859,24 +3869,24 @@
         <v>112</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D31" s="53" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B32" s="51" t="s">
         <v>112</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D32" s="53" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1">
@@ -3887,10 +3897,10 @@
         <v>112</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D33" s="53" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
@@ -3904,7 +3914,7 @@
         <v>142</v>
       </c>
       <c r="D34" s="50" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1">
@@ -3915,10 +3925,10 @@
         <v>112</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D35" s="53" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
@@ -3929,10 +3939,10 @@
         <v>112</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D36" s="53" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1">
@@ -3943,10 +3953,10 @@
         <v>112</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D37" s="53" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1">
@@ -3957,10 +3967,10 @@
         <v>112</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D38" s="53" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1">
@@ -3971,10 +3981,10 @@
         <v>112</v>
       </c>
       <c r="C39" s="50" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D39" s="53" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1">
@@ -3988,7 +3998,7 @@
         <v>143</v>
       </c>
       <c r="D40" s="50" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1">
@@ -3999,10 +4009,10 @@
         <v>112</v>
       </c>
       <c r="C41" s="50" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D41" s="53" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
@@ -4013,10 +4023,10 @@
         <v>112</v>
       </c>
       <c r="C42" s="50" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D42" s="53" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1">
@@ -4027,10 +4037,10 @@
         <v>112</v>
       </c>
       <c r="C43" s="50" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D43" s="53" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1">
@@ -4044,7 +4054,7 @@
         <v>144</v>
       </c>
       <c r="D44" s="50" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1">
@@ -4055,24 +4065,24 @@
         <v>112</v>
       </c>
       <c r="C45" s="50" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D45" s="53" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B46" s="51" t="s">
         <v>112</v>
       </c>
       <c r="C46" s="50" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D46" s="53" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
@@ -4083,10 +4093,10 @@
         <v>112</v>
       </c>
       <c r="C47" s="50" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D47" s="53" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1">
@@ -4097,10 +4107,10 @@
         <v>112</v>
       </c>
       <c r="C48" s="50" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D48" s="53" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1">
@@ -4111,10 +4121,10 @@
         <v>112</v>
       </c>
       <c r="C49" s="50" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D49" s="53" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
@@ -4125,10 +4135,10 @@
         <v>112</v>
       </c>
       <c r="C50" s="50" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D50" s="53" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1">
@@ -4139,10 +4149,10 @@
         <v>146</v>
       </c>
       <c r="C51" s="53" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D51" s="53" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1">
@@ -4152,16 +4162,16 @@
       <c r="B52" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="50" t="s">
-        <v>160</v>
+      <c r="C52" s="55" t="s">
+        <v>274</v>
       </c>
       <c r="D52" s="50" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" s="50" t="s">
         <v>92</v>
@@ -4169,13 +4179,13 @@
       <c r="C53" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="D53" s="53" t="s">
-        <v>190</v>
+      <c r="D53" s="55" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B54" s="51" t="s">
         <v>146</v>
@@ -4183,97 +4193,97 @@
       <c r="C54" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="D54" s="53" t="s">
-        <v>191</v>
+      <c r="D54" s="55" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B55" s="50" t="s">
         <v>108</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D55" s="53" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B56" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="52" t="s">
-        <v>175</v>
+      <c r="C56" s="55" t="s">
+        <v>275</v>
       </c>
       <c r="D56" s="50" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B57" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="52" t="s">
-        <v>176</v>
+      <c r="C57" s="55" t="s">
+        <v>276</v>
       </c>
       <c r="D57" s="50" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B58" s="50" t="s">
         <v>92</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D58" s="50" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" s="51" t="s">
         <v>146</v>
       </c>
       <c r="C59" s="52" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D59" s="50" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B60" s="51" t="s">
         <v>148</v>
       </c>
       <c r="C60" s="54" t="s">
-        <v>276</v>
-      </c>
-      <c r="D60" s="53" t="s">
-        <v>197</v>
+        <v>273</v>
+      </c>
+      <c r="D60" s="55" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B61" s="51" t="s">
         <v>146</v>
@@ -4281,8 +4291,8 @@
       <c r="C61" s="50" t="s">
         <v>157</v>
       </c>
-      <c r="D61" s="50" t="s">
-        <v>196</v>
+      <c r="D61" s="55" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>